<commit_message>
Split out tables.  Employment, Volunteer, Charity
</commit_message>
<xml_diff>
--- a/Personal-Records-Organizer.xlsx
+++ b/Personal-Records-Organizer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId3"/>
@@ -18,13 +18,16 @@
     <sheet name="Military Service" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="Employment" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="Volunteer" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="Bank Accounts and Investments" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="Real Estate" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="Personal Propery" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="Digital Assets" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="Scheduled Payments" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="Debtors and Creditors" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="Insurance" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="Charitable Gifts" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="Safety Deposit" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="Bank Accounts and Investments" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="Real Estate" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="Personal Propery" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="Vehicles" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="Digital Assets" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="Scheduled Payments" sheetId="18" state="visible" r:id="rId20"/>
+    <sheet name="Debtors and Creditors" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="Insurance" sheetId="20" state="visible" r:id="rId22"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="265">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -134,6 +137,9 @@
     <t xml:space="preserve">Other (Specify)</t>
   </si>
   <si>
+    <t xml:space="preserve">Document</t>
+  </si>
+  <si>
     <t xml:space="preserve">Have? (Y/N)</t>
   </si>
   <si>
@@ -299,9 +305,33 @@
     <t xml:space="preserve">Information Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Amount </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Will</t>
+  </si>
+  <si>
     <t xml:space="preserve">Filing Cabinet\</t>
   </si>
   <si>
+    <t xml:space="preserve">Safe Deposit Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Box Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of others with access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keys are located</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contents List located</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type of Account</t>
   </si>
   <si>
@@ -380,9 +410,6 @@
     <t xml:space="preserve">Auto Invest?</t>
   </si>
   <si>
-    <t xml:space="preserve">Frequency</t>
-  </si>
-  <si>
     <t xml:space="preserve">Account paid from</t>
   </si>
   <si>
@@ -530,6 +557,21 @@
     <t xml:space="preserve">manu@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Jewelry / Art / Valuables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurance Policy Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill of sale location</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vehicles</t>
   </si>
   <si>
@@ -542,18 +584,6 @@
     <t xml:space="preserve">Own or Lease</t>
   </si>
   <si>
-    <t xml:space="preserve">Legal document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registration location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insurance Policy Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill of sale location</t>
-  </si>
-  <si>
     <t xml:space="preserve">Truck</t>
   </si>
   <si>
@@ -576,24 +606,6 @@
   </si>
   <si>
     <t xml:space="preserve">own</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jewelry / Art / Valuables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safe Deposit Box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Box Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of others with access</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keys are located</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contents List located</t>
   </si>
   <si>
     <t xml:space="preserve">Password Management</t>
@@ -1171,7 +1183,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1213,10 +1225,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1226,18 +1238,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -1251,7 +1263,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1999</v>
@@ -1260,54 +1272,21 @@
         <v>2000</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1324,9 +1303,163 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1" style="0" width="12.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:D1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="9" style="0" width="12.64"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1340,13 +1473,13 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
@@ -1360,41 +1493,41 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
@@ -1407,39 +1540,39 @@
         <v>18</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>123</v>
@@ -1447,37 +1580,37 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,18 +1633,18 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="7" t="s">
@@ -1524,34 +1657,34 @@
         <v>18</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1559,13 +1692,13 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1576,7 +1709,7 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1584,13 +1717,13 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1601,7 +1734,7 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1609,7 +1742,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>21</v>
@@ -1624,7 +1757,7 @@
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1643,7 +1776,7 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1661,18 +1794,18 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="7" t="s">
@@ -1685,34 +1818,34 @@
         <v>18</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="L20" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N20" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="M20" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="O20" s="7" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1720,13 +1853,13 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1737,23 +1870,23 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1766,29 +1899,29 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1798,47 +1931,47 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,12 +1984,12 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1871,50 +2004,50 @@
         <v>18</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1928,7 +2061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1946,22 +2079,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>17</v>
@@ -1970,119 +2103,119 @@
         <v>18</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2096,15 +2229,90 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="9" style="0" width="12.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2122,130 +2330,106 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>180</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>171</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>181</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>185</v>
-      </c>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2258,7 +2442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2276,38 +2460,38 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>123</v>
@@ -2315,16 +2499,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>123</v>
@@ -2332,177 +2516,177 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>123456780</v>
@@ -2538,7 +2722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2556,13 +2740,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
@@ -2574,33 +2758,33 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>123</v>
@@ -2609,20 +2793,20 @@
         <v>100</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="7" t="s">
@@ -2635,26 +2819,26 @@
         <v>18</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="7" t="s">
@@ -2667,13 +2851,13 @@
         <v>18</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2687,14 +2871,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2708,13 +2892,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
@@ -2726,36 +2910,36 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>123</v>
@@ -2818,13 +3002,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -2836,36 +3020,36 @@
         <v>18</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>123</v>
@@ -2928,18 +3112,18 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2953,7 +3137,107 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="2" style="0" width="12.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2981,16 +3265,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>16</v>
@@ -3002,85 +3286,85 @@
         <v>18</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>16</v>
@@ -3092,35 +3376,35 @@
         <v>18</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>16</v>
@@ -3132,41 +3416,41 @@
         <v>18</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>16</v>
@@ -3178,123 +3462,23 @@
         <v>18</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="2" style="0" width="12.64"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3314,7 +3498,7 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3491,7 +3675,7 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3685,8 +3869,8 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3701,23 +3885,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -3729,114 +3916,114 @@
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>36161</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>36161</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>36161</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -3862,7 +4049,7 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3874,18 +4061,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3898,7 +4085,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3906,79 +4093,79 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3999,7 +4186,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4011,18 +4198,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4038,7 +4225,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4046,15 +4233,15 @@
         <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -4075,7 +4262,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4087,23 +4274,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>123</v>
@@ -4111,10 +4298,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4135,7 +4322,7 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4146,7 +4333,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,10 +4341,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -4171,7 +4358,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1999</v>
@@ -4180,13 +4367,13 @@
         <v>2000</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split many tabs that became one table that should have been multiple.  Added Modal, Model, DB, Admin etc
</commit_message>
<xml_diff>
--- a/Personal-Records-Organizer.xlsx
+++ b/Personal-Records-Organizer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,8 +26,10 @@
     <sheet name="Vehicles" sheetId="16" state="visible" r:id="rId18"/>
     <sheet name="Digital Assets" sheetId="17" state="visible" r:id="rId19"/>
     <sheet name="Scheduled Payments" sheetId="18" state="visible" r:id="rId20"/>
-    <sheet name="Debtors and Creditors" sheetId="19" state="visible" r:id="rId21"/>
-    <sheet name="Insurance" sheetId="20" state="visible" r:id="rId22"/>
+    <sheet name="Creditors" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="Debtors" sheetId="20" state="visible" r:id="rId22"/>
+    <sheet name="Contracts" sheetId="21" state="visible" r:id="rId23"/>
+    <sheet name="Insurance" sheetId="22" state="visible" r:id="rId24"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1459,7 +1461,7 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2068,7 +2070,7 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2237,7 +2239,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2449,7 +2451,7 @@
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2729,7 +2731,7 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2876,10 +2878,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3000,132 +3002,23 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="3" t="n">
-        <v>123</v>
-      </c>
-      <c r="H14" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="I14" s="11" t="n">
-        <v>36526</v>
-      </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3242,9 +3135,238 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:J1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="4" style="0" width="12.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="H2" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="I2" s="11" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="4" style="0" width="12.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>